<commit_message>
changes to existing files
</commit_message>
<xml_diff>
--- a/ANSWER-Veda Migration Log.xlsx
+++ b/ANSWER-Veda Migration Log.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIM-EL\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67347728-826A-4C3E-93DA-3E96BBE0DDFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80AE29E5-8CA2-405B-8C5F-D6F5EA0037A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14670" yWindow="-16830" windowWidth="19335" windowHeight="14265" xr2:uid="{010DEB55-B266-4EDB-AF61-05BEFBEEB6AD}"/>
+    <workbookView xWindow="9465" yWindow="1335" windowWidth="19335" windowHeight="14265" xr2:uid="{010DEB55-B266-4EDB-AF61-05BEFBEEB6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Migration Log</t>
   </si>
@@ -84,6 +84,27 @@
   </si>
   <si>
     <t>FLO_EFF-I-&gt;CEFF-I</t>
+  </si>
+  <si>
+    <t>Questions for Amit</t>
+  </si>
+  <si>
+    <t>FLO_EMISS?</t>
+  </si>
+  <si>
+    <t>COM_PROJ?</t>
+  </si>
+  <si>
+    <t>GAMS Engine credentials?</t>
+  </si>
+  <si>
+    <t>VO setup - linking to Git.</t>
+  </si>
+  <si>
+    <t>Is it possible to initiate the VO run from the command prompt?</t>
+  </si>
+  <si>
+    <t>Does the user get access to the GDX file when run is done?</t>
   </si>
 </sst>
 </file>
@@ -482,10 +503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69140962-8DE1-4028-A4EB-D25405C99763}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,6 +602,41 @@
         <v>15</v>
       </c>
     </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>